<commit_message>
2022 12 21 16
</commit_message>
<xml_diff>
--- a/pengaduan-bpbd.xlsx
+++ b/pengaduan-bpbd.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE" sheetId="1" r:id="rId1"/>
     <sheet name="INSERT WILAYAH" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="171">
   <si>
     <t>user</t>
   </si>
@@ -530,12 +530,15 @@
   </si>
   <si>
     <t>WEDUSAN</t>
+  </si>
+  <si>
+    <t>bukti_peninjauan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -919,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1121,6 +1124,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="1:13">
+      <c r="G10" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1131,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="D130" sqref="D130"/>
+    <sheetView topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123:E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
2022 12 02 16:02
</commit_message>
<xml_diff>
--- a/pengaduan-bpbd.xlsx
+++ b/pengaduan-bpbd.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE" sheetId="1" r:id="rId1"/>
     <sheet name="INSERT WILAYAH" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="169">
   <si>
     <t>user</t>
   </si>
@@ -415,87 +415,6 @@
     <t>AGUNGMULYO</t>
   </si>
   <si>
-    <t> BAJOMULYO</t>
-  </si>
-  <si>
-    <t> BAKARAN KULON</t>
-  </si>
-  <si>
-    <t> BAKARAN WETAN</t>
-  </si>
-  <si>
-    <t> BENDAR</t>
-  </si>
-  <si>
-    <t> BRINGIN</t>
-  </si>
-  <si>
-    <t> BUMIREJO</t>
-  </si>
-  <si>
-    <t> DOROPAYUNG</t>
-  </si>
-  <si>
-    <t> DUKUTALIT</t>
-  </si>
-  <si>
-    <t> GADINGREJO</t>
-  </si>
-  <si>
-    <t> GENENGMULYO</t>
-  </si>
-  <si>
-    <t> GROWONG KIDUL</t>
-  </si>
-  <si>
-    <t> GROWONG LOR</t>
-  </si>
-  <si>
-    <t> JEPURO</t>
-  </si>
-  <si>
-    <t> KARANG</t>
-  </si>
-  <si>
-    <t> KARANGREJO</t>
-  </si>
-  <si>
-    <t> KAUMAN</t>
-  </si>
-  <si>
-    <t> KEBONSAWAHAN</t>
-  </si>
-  <si>
-    <t> KEDUNGPANCING</t>
-  </si>
-  <si>
-    <t> KETIP</t>
-  </si>
-  <si>
-    <t> KUDUKERAS</t>
-  </si>
-  <si>
-    <t> LANGENHARJO</t>
-  </si>
-  <si>
-    <t> MARGOMULYO</t>
-  </si>
-  <si>
-    <t> MINTOMULYO</t>
-  </si>
-  <si>
-    <t> PAJEKSAN</t>
-  </si>
-  <si>
-    <t> PEKUWON</t>
-  </si>
-  <si>
-    <t> SEJOMULYO</t>
-  </si>
-  <si>
-    <t> TLUWAH</t>
-  </si>
-  <si>
     <t>BAKALAN</t>
   </si>
   <si>
@@ -533,6 +452,81 @@
   </si>
   <si>
     <t>bukti_peninjauan</t>
+  </si>
+  <si>
+    <t>BAJOMULYO</t>
+  </si>
+  <si>
+    <t>BAKARAN KULON</t>
+  </si>
+  <si>
+    <t>BAKARAN WETAN</t>
+  </si>
+  <si>
+    <t>BENDAR</t>
+  </si>
+  <si>
+    <t>BRINGIN</t>
+  </si>
+  <si>
+    <t>DOROPAYUNG</t>
+  </si>
+  <si>
+    <t>DUKUTALIT</t>
+  </si>
+  <si>
+    <t>GADINGREJO</t>
+  </si>
+  <si>
+    <t>GENENGMULYO</t>
+  </si>
+  <si>
+    <t>GROWONG KIDUL</t>
+  </si>
+  <si>
+    <t>GROWONG LOR</t>
+  </si>
+  <si>
+    <t>JEPURO</t>
+  </si>
+  <si>
+    <t>KARANG</t>
+  </si>
+  <si>
+    <t>KARANGREJO</t>
+  </si>
+  <si>
+    <t>KAUMAN</t>
+  </si>
+  <si>
+    <t>KEBONSAWAHAN</t>
+  </si>
+  <si>
+    <t>KEDUNGPANCING</t>
+  </si>
+  <si>
+    <t>KETIP</t>
+  </si>
+  <si>
+    <t>KUDUKERAS</t>
+  </si>
+  <si>
+    <t>MARGOMULYO</t>
+  </si>
+  <si>
+    <t>MINTOMULYO</t>
+  </si>
+  <si>
+    <t>PAJEKSAN</t>
+  </si>
+  <si>
+    <t>PEKUWON</t>
+  </si>
+  <si>
+    <t>SEJOMULYO</t>
+  </si>
+  <si>
+    <t>TLUWAH</t>
   </si>
 </sst>
 </file>
@@ -924,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1126,7 +1120,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="G10" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1139,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q137"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
       <selection activeCell="E123" sqref="E123:E134"/>
     </sheetView>
   </sheetViews>
@@ -2822,18 +2816,18 @@
         <v>2</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C94" s="5">
         <v>59185</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" ref="E94:E120" si="6">"INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','"&amp;B94&amp;"','"&amp;C94&amp;"');"</f>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' BAJOMULYO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','BAJOMULYO','59185');</v>
       </c>
       <c r="Q94" t="str">
         <f t="shared" si="4"/>
-        <v> BAJOMULYO</v>
+        <v>BAJOMULYO</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="15.75" thickBot="1">
@@ -2841,18 +2835,18 @@
         <v>3</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C95" s="5">
         <v>59185</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' BAKARAN KULON','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','BAKARAN KULON','59185');</v>
       </c>
       <c r="Q95" t="str">
         <f t="shared" si="4"/>
-        <v> BAKARAN KULON</v>
+        <v>BAKARAN KULON</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="15.75" thickBot="1">
@@ -2860,18 +2854,18 @@
         <v>4</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="C96" s="5">
         <v>59185</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' BAKARAN WETAN','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','BAKARAN WETAN','59185');</v>
       </c>
       <c r="Q96" t="str">
         <f t="shared" si="4"/>
-        <v> BAKARAN WETAN</v>
+        <v>BAKARAN WETAN</v>
       </c>
     </row>
     <row r="97" spans="1:17" ht="15.75" thickBot="1">
@@ -2879,18 +2873,18 @@
         <v>5</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C97" s="5">
         <v>59185</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' BENDAR','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','BENDAR','59185');</v>
       </c>
       <c r="Q97" t="str">
         <f t="shared" si="4"/>
-        <v> BENDAR</v>
+        <v>BENDAR</v>
       </c>
     </row>
     <row r="98" spans="1:17" ht="15.75" thickBot="1">
@@ -2898,18 +2892,18 @@
         <v>6</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C98" s="5">
         <v>59185</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' BRINGIN','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','BRINGIN','59185');</v>
       </c>
       <c r="Q98" t="str">
         <f t="shared" si="4"/>
-        <v> BRINGIN</v>
+        <v>BRINGIN</v>
       </c>
     </row>
     <row r="99" spans="1:17" ht="15.75" thickBot="1">
@@ -2917,18 +2911,18 @@
         <v>7</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="C99" s="5">
         <v>59185</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' BUMIREJO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','BUMIREJO','59185');</v>
       </c>
       <c r="Q99" t="str">
         <f t="shared" si="4"/>
-        <v> BUMIREJO</v>
+        <v>BUMIREJO</v>
       </c>
     </row>
     <row r="100" spans="1:17" ht="15.75" thickBot="1">
@@ -2936,18 +2930,18 @@
         <v>8</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C100" s="5">
         <v>59185</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' DOROPAYUNG','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','DOROPAYUNG','59185');</v>
       </c>
       <c r="Q100" t="str">
         <f t="shared" si="4"/>
-        <v> DOROPAYUNG</v>
+        <v>DOROPAYUNG</v>
       </c>
     </row>
     <row r="101" spans="1:17" ht="15.75" thickBot="1">
@@ -2955,18 +2949,18 @@
         <v>9</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="C101" s="5">
         <v>59185</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' DUKUTALIT','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','DUKUTALIT','59185');</v>
       </c>
       <c r="Q101" t="str">
         <f t="shared" si="4"/>
-        <v> DUKUTALIT</v>
+        <v>DUKUTALIT</v>
       </c>
     </row>
     <row r="102" spans="1:17" ht="15.75" thickBot="1">
@@ -2974,18 +2968,18 @@
         <v>10</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C102" s="5">
         <v>59185</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' GADINGREJO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','GADINGREJO','59185');</v>
       </c>
       <c r="Q102" t="str">
         <f t="shared" si="4"/>
-        <v> GADINGREJO</v>
+        <v>GADINGREJO</v>
       </c>
     </row>
     <row r="103" spans="1:17" ht="15.75" thickBot="1">
@@ -2993,18 +2987,18 @@
         <v>11</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C103" s="5">
         <v>59185</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' GENENGMULYO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','GENENGMULYO','59185');</v>
       </c>
       <c r="Q103" t="str">
         <f t="shared" si="4"/>
-        <v> GENENGMULYO</v>
+        <v>GENENGMULYO</v>
       </c>
     </row>
     <row r="104" spans="1:17" ht="15.75" thickBot="1">
@@ -3012,18 +3006,18 @@
         <v>12</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="C104" s="5">
         <v>59185</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' GROWONG KIDUL','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','GROWONG KIDUL','59185');</v>
       </c>
       <c r="Q104" t="str">
         <f t="shared" si="4"/>
-        <v> GROWONG KIDUL</v>
+        <v>GROWONG KIDUL</v>
       </c>
     </row>
     <row r="105" spans="1:17" ht="15.75" thickBot="1">
@@ -3031,18 +3025,18 @@
         <v>13</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="C105" s="5">
         <v>59185</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' GROWONG LOR','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','GROWONG LOR','59185');</v>
       </c>
       <c r="Q105" t="str">
         <f t="shared" si="4"/>
-        <v> GROWONG LOR</v>
+        <v>GROWONG LOR</v>
       </c>
     </row>
     <row r="106" spans="1:17" ht="15.75" thickBot="1">
@@ -3050,18 +3044,18 @@
         <v>14</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C106" s="5">
         <v>59185</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' JEPURO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','JEPURO','59185');</v>
       </c>
       <c r="Q106" t="str">
         <f t="shared" si="4"/>
-        <v> JEPURO</v>
+        <v>JEPURO</v>
       </c>
     </row>
     <row r="107" spans="1:17" ht="15.75" thickBot="1">
@@ -3069,18 +3063,18 @@
         <v>15</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="C107" s="5">
         <v>59185</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' KARANG','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','KARANG','59185');</v>
       </c>
       <c r="Q107" t="str">
         <f t="shared" si="4"/>
-        <v> KARANG</v>
+        <v>KARANG</v>
       </c>
     </row>
     <row r="108" spans="1:17" ht="15.75" thickBot="1">
@@ -3088,18 +3082,18 @@
         <v>16</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C108" s="5">
         <v>59185</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' KARANGREJO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','KARANGREJO','59185');</v>
       </c>
       <c r="Q108" t="str">
         <f t="shared" si="4"/>
-        <v> KARANGREJO</v>
+        <v>KARANGREJO</v>
       </c>
     </row>
     <row r="109" spans="1:17" ht="15.75" thickBot="1">
@@ -3107,18 +3101,18 @@
         <v>17</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="C109" s="5">
         <v>59185</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' KAUMAN','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','KAUMAN','59185');</v>
       </c>
       <c r="Q109" t="str">
         <f t="shared" si="4"/>
-        <v> KAUMAN</v>
+        <v>KAUMAN</v>
       </c>
     </row>
     <row r="110" spans="1:17" ht="15.75" thickBot="1">
@@ -3126,18 +3120,18 @@
         <v>18</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C110" s="5">
         <v>59185</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' KEBONSAWAHAN','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','KEBONSAWAHAN','59185');</v>
       </c>
       <c r="Q110" t="str">
         <f t="shared" si="4"/>
-        <v> KEBONSAWAHAN</v>
+        <v>KEBONSAWAHAN</v>
       </c>
     </row>
     <row r="111" spans="1:17" ht="15.75" thickBot="1">
@@ -3145,18 +3139,18 @@
         <v>19</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="C111" s="5">
         <v>59185</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' KEDUNGPANCING','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','KEDUNGPANCING','59185');</v>
       </c>
       <c r="Q111" t="str">
         <f t="shared" si="4"/>
-        <v> KEDUNGPANCING</v>
+        <v>KEDUNGPANCING</v>
       </c>
     </row>
     <row r="112" spans="1:17" ht="15.75" thickBot="1">
@@ -3164,18 +3158,18 @@
         <v>20</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="C112" s="5">
         <v>59185</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' KETIP','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','KETIP','59185');</v>
       </c>
       <c r="Q112" t="str">
         <f t="shared" si="4"/>
-        <v> KETIP</v>
+        <v>KETIP</v>
       </c>
     </row>
     <row r="113" spans="1:17" ht="15.75" thickBot="1">
@@ -3183,18 +3177,18 @@
         <v>21</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="C113" s="5">
         <v>59185</v>
       </c>
       <c r="E113" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' KUDUKERAS','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','KUDUKERAS','59185');</v>
       </c>
       <c r="Q113" t="str">
         <f t="shared" si="4"/>
-        <v> KUDUKERAS</v>
+        <v>KUDUKERAS</v>
       </c>
     </row>
     <row r="114" spans="1:17" ht="15.75" thickBot="1">
@@ -3202,18 +3196,18 @@
         <v>22</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="C114" s="5">
         <v>59185</v>
       </c>
       <c r="E114" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' LANGENHARJO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','LANGENHARJO','59185');</v>
       </c>
       <c r="Q114" t="str">
         <f t="shared" si="4"/>
-        <v> LANGENHARJO</v>
+        <v>LANGENHARJO</v>
       </c>
     </row>
     <row r="115" spans="1:17" ht="15.75" thickBot="1">
@@ -3221,18 +3215,18 @@
         <v>23</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C115" s="5">
         <v>59185</v>
       </c>
       <c r="E115" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' MARGOMULYO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','MARGOMULYO','59185');</v>
       </c>
       <c r="Q115" t="str">
         <f t="shared" si="4"/>
-        <v> MARGOMULYO</v>
+        <v>MARGOMULYO</v>
       </c>
     </row>
     <row r="116" spans="1:17" ht="15.75" thickBot="1">
@@ -3240,18 +3234,18 @@
         <v>24</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C116" s="5">
         <v>59185</v>
       </c>
       <c r="E116" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' MINTOMULYO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','MINTOMULYO','59185');</v>
       </c>
       <c r="Q116" t="str">
         <f t="shared" si="4"/>
-        <v> MINTOMULYO</v>
+        <v>MINTOMULYO</v>
       </c>
     </row>
     <row r="117" spans="1:17" ht="15.75" thickBot="1">
@@ -3259,18 +3253,18 @@
         <v>25</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="C117" s="5">
         <v>59185</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' PAJEKSAN','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','PAJEKSAN','59185');</v>
       </c>
       <c r="Q117" t="str">
         <f t="shared" si="4"/>
-        <v> PAJEKSAN</v>
+        <v>PAJEKSAN</v>
       </c>
     </row>
     <row r="118" spans="1:17" ht="15.75" thickBot="1">
@@ -3278,18 +3272,18 @@
         <v>26</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="C118" s="5">
         <v>59185</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' PEKUWON','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','PEKUWON','59185');</v>
       </c>
       <c r="Q118" t="str">
         <f t="shared" si="4"/>
-        <v> PEKUWON</v>
+        <v>PEKUWON</v>
       </c>
     </row>
     <row r="119" spans="1:17" ht="15.75" thickBot="1">
@@ -3297,18 +3291,18 @@
         <v>27</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C119" s="5">
         <v>59185</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' SEJOMULYO','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','SEJOMULYO','59185');</v>
       </c>
       <c r="Q119" t="str">
         <f t="shared" si="4"/>
-        <v> SEJOMULYO</v>
+        <v>SEJOMULYO</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="15.75" thickBot="1">
@@ -3316,24 +3310,21 @@
         <v>28</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="C120" s="5">
         <v>59185</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA',' TLUWAH','59185');</v>
+        <v>INSERT INTO wilayah (kecamatan, desa, no_telp) VALUES ('JUWANA','TLUWAH','59185');</v>
       </c>
       <c r="Q120" t="str">
         <f t="shared" si="4"/>
-        <v> TLUWAH</v>
+        <v>TLUWAH</v>
       </c>
     </row>
     <row r="121" spans="1:17">
-      <c r="B121" t="s">
-        <v>79</v>
-      </c>
       <c r="Q121" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3353,7 +3344,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="C123" s="5">
         <v>59158</v>
@@ -3372,7 +3363,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C124" s="5">
         <v>59158</v>
@@ -3391,7 +3382,7 @@
         <v>3</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="C125" s="5">
         <v>59158</v>
@@ -3410,7 +3401,7 @@
         <v>4</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C126" s="5">
         <v>59158</v>
@@ -3429,7 +3420,7 @@
         <v>5</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="C127" s="5">
         <v>59158</v>
@@ -3448,7 +3439,7 @@
         <v>6</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="C128" s="5">
         <v>59158</v>
@@ -3467,7 +3458,7 @@
         <v>7</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="C129" s="5">
         <v>59158</v>
@@ -3486,7 +3477,7 @@
         <v>8</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="C130" s="5">
         <v>59158</v>
@@ -3505,7 +3496,7 @@
         <v>9</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="C131" s="5">
         <v>59158</v>
@@ -3524,7 +3515,7 @@
         <v>10</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="C132" s="5">
         <v>59158</v>
@@ -3543,7 +3534,7 @@
         <v>11</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="C133" s="5">
         <v>59158</v>
@@ -3562,7 +3553,7 @@
         <v>12</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="C134" s="5">
         <v>59158</v>

</xml_diff>

<commit_message>
2023 01 05 15:48
</commit_message>
<xml_diff>
--- a/pengaduan-bpbd.xlsx
+++ b/pengaduan-bpbd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE" sheetId="1" r:id="rId1"/>
@@ -1114,7 +1114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1265,8 +1265,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1275,67 +1275,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1438,251 +1378,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5125,8 +4825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5151,8 +4851,8 @@
         <v>339</v>
       </c>
       <c r="D2" t="str">
-        <f>"INSERT bencana (id_bencana, nama_bencana) VALUES ("&amp;A2&amp;", '"&amp;B2&amp;"');"</f>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (1, 'Banjir');</v>
+        <f>"INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES ("&amp;A2&amp;", '"&amp;B2&amp;"');"</f>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (1, 'Banjir');</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5163,8 +4863,8 @@
         <v>208</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D25" si="0">"INSERT bencana (id_bencana, nama_bencana) VALUES ("&amp;A3&amp;", '"&amp;B3&amp;"');"</f>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (2, 'Tanah Longsor');</v>
+        <f t="shared" ref="D3:D25" si="0">"INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES ("&amp;A3&amp;", '"&amp;B3&amp;"');"</f>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (2, 'Tanah Longsor');</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5176,7 +4876,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (3, 'Banjir dan Tanah longsor');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (3, 'Banjir dan Tanah longsor');</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5188,7 +4888,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (4, 'Abrasi');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (4, 'Abrasi');</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5200,7 +4900,7 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (5, 'Puting Beliung');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (5, 'Puting Beliung');</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5212,7 +4912,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (6, 'Kekeringan');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (6, 'Kekeringan');</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5224,7 +4924,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (7, 'Kebakaran');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (7, 'Kebakaran');</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5236,7 +4936,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (8, 'Kebakaran Hutan dan Lahan');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (8, 'Kebakaran Hutan dan Lahan');</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5248,7 +4948,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (9, 'Gempa Bumi');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (9, 'Gempa Bumi');</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5260,7 +4960,7 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (10, 'Tsunami');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (10, 'Tsunami');</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5272,7 +4972,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (11, 'Gempa Bumi dan Tsunami');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (11, 'Gempa Bumi dan Tsunami');</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5284,7 +4984,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (12, 'Letusan Gunung Api');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (12, 'Letusan Gunung Api');</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5296,7 +4996,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (13, 'Wabah Penyakit');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (13, 'Wabah Penyakit');</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5308,7 +5008,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (14, 'Pohon Tumbang');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (14, 'Pohon Tumbang');</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5320,7 +5020,7 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (15, 'Angin Kencang');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (15, 'Angin Kencang');</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5332,7 +5032,7 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (16, 'Rumah Tertimpa Pohon Akibat Angin Kencang Disertai Hujan Deras');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (16, 'Rumah Tertimpa Pohon Akibat Angin Kencang Disertai Hujan Deras');</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5344,7 +5044,7 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (17, 'Pohon Tumbang');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (17, 'Pohon Tumbang');</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5356,7 +5056,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (18, 'Orang Tenggelam');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (18, 'Orang Tenggelam');</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5368,7 +5068,7 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (19, 'Pondokan Roboh');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (19, 'Pondokan Roboh');</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5380,7 +5080,7 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (20, 'Kebakaran Rumah');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (20, 'Kebakaran Rumah');</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5392,7 +5092,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (21, 'Evakuasi Sarang Tawon');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (21, 'Evakuasi Sarang Tawon');</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5404,7 +5104,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (22, 'Tebing Longsor');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (22, 'Tebing Longsor');</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5416,7 +5116,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (23, 'Orang Hilang di perairan ( Hilang Kontak )');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (23, 'Orang Hilang di perairan ( Hilang Kontak )');</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5428,7 +5128,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT bencana (id_bencana, nama_bencana) VALUES (24, 'Lainnya');</v>
+        <v>INSERT INTO `bencana`(`id_bencana`, `nama_bencana`) VALUES (24, 'Lainnya');</v>
       </c>
     </row>
   </sheetData>
@@ -5440,8 +5140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5469,8 +5169,8 @@
         <v>321</v>
       </c>
       <c r="D2" t="str">
-        <f>"INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A2&amp;",'"&amp;B2&amp;"','MATERIAL','"&amp;C2&amp;"','[value-5]')"</f>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (1,'Karung Plastik','MATERIAL','Lembar','[value-5]')</v>
+        <f>"INSERT INTO `bantuan`  (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A2&amp;",'"&amp;B2&amp;"','MATERIAL','"&amp;C2&amp;"','YYYYMMDD');"</f>
+        <v>INSERT INTO `bantuan`  (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (1,'Karung Plastik','MATERIAL','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5484,8 +5184,8 @@
         <v>321</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D17" si="0">"INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A3&amp;",'"&amp;B3&amp;"','MATERIAL','"&amp;C3&amp;"','[value-5]')"</f>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (2,'Triplek','MATERIAL','Lembar','[value-5]')</v>
+        <f>"INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A3&amp;",'"&amp;B3&amp;"','MATERIAL','"&amp;C3&amp;"','YYYYMMDD');"</f>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (2,'Triplek','MATERIAL','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5499,8 +5199,8 @@
         <v>321</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (3,'Seng','MATERIAL','Lembar','[value-5]')</v>
+        <f t="shared" ref="D3:D17" si="0">"INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A4&amp;",'"&amp;B4&amp;"','MATERIAL','"&amp;C4&amp;"','YYYYMMDD');"</f>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (3,'Seng','MATERIAL','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5515,7 +5215,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (4,'Paku Payung','MATERIAL','Ons','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (4,'Paku Payung','MATERIAL','Ons','YYYYMMDD');</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5530,7 +5230,7 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (5,'Paku Usuk','MATERIAL','Ons','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (5,'Paku Usuk','MATERIAL','Ons','YYYYMMDD');</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5545,7 +5245,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (6,'Paku Reng','MATERIAL','Ons','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (6,'Paku Reng','MATERIAL','Ons','YYYYMMDD');</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5560,7 +5260,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (7,'Tanah Urug','MATERIAL','m³','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (7,'Tanah Urug','MATERIAL','m³','YYYYMMDD');</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5575,7 +5275,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (8,'Kawat Bronjong','MATERIAL','Biji','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (8,'Kawat Bronjong','MATERIAL','Biji','YYYYMMDD');</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5590,7 +5290,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (9,'Batu Belah','MATERIAL','m³','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (9,'Batu Belah','MATERIAL','m³','YYYYMMDD');</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5605,7 +5305,7 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (10,'Seng Bergelombang','MATERIAL','Lembar','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (10,'Seng Bergelombang','MATERIAL','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5620,7 +5320,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (11,'Plastik Mika Penutup Longsor','MATERIAL','Roll','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (11,'Plastik Mika Penutup Longsor','MATERIAL','Roll','YYYYMMDD');</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5635,7 +5335,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (12,'Genteng','MATERIAL','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (12,'Genteng','MATERIAL','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5650,7 +5350,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (13,'Kerpus','MATERIAL','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (13,'Kerpus','MATERIAL','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5665,7 +5365,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (14,'Semen','MATERIAL','Sak','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (14,'Semen','MATERIAL','Sak','YYYYMMDD');</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5680,7 +5380,7 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (15,'Batu Bata','MATERIAL','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (15,'Batu Bata','MATERIAL','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5694,8 +5394,8 @@
         <v>323</v>
       </c>
       <c r="D17" t="str">
-        <f>"INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A17&amp;",'"&amp;B17&amp;"','MATERIAL','"&amp;C17&amp;"','[value-5]')"</f>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (16,'Pasir','MATERIAL','m³','[value-5]')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (16,'Pasir','MATERIAL','m³','YYYYMMDD');</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5714,8 +5414,8 @@
         <v>321</v>
       </c>
       <c r="D20" t="str">
-        <f>"INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A20&amp;",'"&amp;B20&amp;"','SANDANG','"&amp;C20&amp;"','[value-5]')"</f>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (17,'Selimut','SANDANG','Lembar','[value-5]')</v>
+        <f>"INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A20&amp;",'"&amp;B20&amp;"','SANDANG','"&amp;C20&amp;"','YYYYMMDD');"</f>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (17,'Selimut','SANDANG','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5729,8 +5429,8 @@
         <v>321</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" ref="D21:D84" si="1">"INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A21&amp;",'"&amp;B21&amp;"','SANDANG','"&amp;C21&amp;"','[value-5]')"</f>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (18,'Selimut Lurik','SANDANG','Lembar','[value-5]')</v>
+        <f t="shared" ref="D21:D84" si="1">"INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A21&amp;",'"&amp;B21&amp;"','SANDANG','"&amp;C21&amp;"','YYYYMMDD');"</f>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (18,'Selimut Lurik','SANDANG','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5745,7 +5445,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (19,'Jarik','SANDANG','Lembar','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (19,'Jarik','SANDANG','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5760,7 +5460,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (20,'Sarung','SANDANG','Lembar','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (20,'Sarung','SANDANG','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5775,7 +5475,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (21,'Kelambu','SANDANG','Lembar','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (21,'Kelambu','SANDANG','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5790,7 +5490,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (22,'Baju anak','SANDANG','Pcs','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (22,'Baju anak','SANDANG','Pcs','YYYYMMDD');</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5805,7 +5505,7 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (23,'Kaos dalam laki - laki ','SANDANG','Pcs','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (23,'Kaos dalam laki - laki ','SANDANG','Pcs','YYYYMMDD');</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5820,7 +5520,7 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (24,'Celana dalam wanita','SANDANG','Pcs','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (24,'Celana dalam wanita','SANDANG','Pcs','YYYYMMDD');</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5835,7 +5535,7 @@
       </c>
       <c r="D28" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (25,'Daster','SANDANG','Pcs','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (25,'Daster','SANDANG','Pcs','YYYYMMDD');</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5850,7 +5550,7 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (26,'Kaos untuk relawan','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (26,'Kaos untuk relawan','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5865,7 +5565,7 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (27,'Seragam Relawan','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (27,'Seragam Relawan','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5880,7 +5580,7 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (28,'Paket Sandang','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (28,'Paket Sandang','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5895,7 +5595,7 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (29,'Kid Ware','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (29,'Kid Ware','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5910,7 +5610,7 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (30,'Kids Ware','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (30,'Kids Ware','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5925,7 +5625,7 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (31,'Family Kit','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (31,'Family Kit','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5940,7 +5640,7 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (32,'Peralatan Dapur / Food ware','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (32,'Peralatan Dapur / Food ware','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -5955,7 +5655,7 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (33,'Peralatan Kesehatan Rumah Tangga','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (33,'Peralatan Kesehatan Rumah Tangga','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -5970,7 +5670,7 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (34,'Peralatan Kesehatan/Kebersihan','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (34,'Peralatan Kesehatan/Kebersihan','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -5985,7 +5685,7 @@
       </c>
       <c r="D38" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (35,'Perlengkapan Sekolah','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (35,'Perlengkapan Sekolah','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -6000,7 +5700,7 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (36,'Perlengkapan Makan','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (36,'Perlengkapan Makan','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -6015,7 +5715,7 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (37,'Kantong Mayat','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (37,'Kantong Mayat','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -6030,7 +5730,7 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (38,'Kantong Jenazah','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (38,'Kantong Jenazah','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -6045,7 +5745,7 @@
       </c>
       <c r="D42" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (39,'Paket Rekreasional','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (39,'Paket Rekreasional','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -6060,7 +5760,7 @@
       </c>
       <c r="D43" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (40,'Medical kit','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (40,'Medical kit','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -6075,7 +5775,7 @@
       </c>
       <c r="D44" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (41,'Matras ','SANDANG','Lembar','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (41,'Matras ','SANDANG','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -6090,7 +5790,7 @@
       </c>
       <c r="D45" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (42,'Tikar ','SANDANG','Lembar','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (42,'Tikar ','SANDANG','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -6105,7 +5805,7 @@
       </c>
       <c r="D46" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (43,'Tenda Gulung','SANDANG','Lembar','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (43,'Tenda Gulung','SANDANG','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -6120,7 +5820,7 @@
       </c>
       <c r="D47" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (44,'Paket Seragam PA','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (44,'Paket Seragam PA','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -6135,7 +5835,7 @@
       </c>
       <c r="D48" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (45,'Paket Seragam PI','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (45,'Paket Seragam PI','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -6150,7 +5850,7 @@
       </c>
       <c r="D49" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (46,'Tas Sekolah','SANDANG','Pcs','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (46,'Tas Sekolah','SANDANG','Pcs','YYYYMMDD');</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -6165,7 +5865,7 @@
       </c>
       <c r="D50" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (47,'Pakaian Seragam SD PA','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (47,'Pakaian Seragam SD PA','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -6180,7 +5880,7 @@
       </c>
       <c r="D51" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (48,'Pakaian Seragam SD PI','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (48,'Pakaian Seragam SD PI','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -6195,7 +5895,7 @@
       </c>
       <c r="D52" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (49,'Handuk','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (49,'Handuk','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -6210,7 +5910,7 @@
       </c>
       <c r="D53" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (50,'Wajan ','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (50,'Wajan ','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -6225,7 +5925,7 @@
       </c>
       <c r="D54" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (51,'Panci ','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (51,'Panci ','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -6240,7 +5940,7 @@
       </c>
       <c r="D55" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (52,'Brosur Kebencanaan','SANDANG','Lembar','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (52,'Brosur Kebencanaan','SANDANG','Lembar','YYYYMMDD');</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -6255,7 +5955,7 @@
       </c>
       <c r="D56" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (53,'Sepatu Boot','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (53,'Sepatu Boot','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -6270,7 +5970,7 @@
       </c>
       <c r="D57" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (54,'Jas Hujan','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (54,'Jas Hujan','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -6285,7 +5985,7 @@
       </c>
       <c r="D58" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (55,'Webbing','SANDANG','Roll','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (55,'Webbing','SANDANG','Roll','YYYYMMDD');</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -6300,7 +6000,7 @@
       </c>
       <c r="D59" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (56,'Buku Cerita','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (56,'Buku Cerita','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -6315,7 +6015,7 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (57,'Buku Saku Kebencanaan','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (57,'Buku Saku Kebencanaan','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -6330,7 +6030,7 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (58,'Tas Tahan Air','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (58,'Tas Tahan Air','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -6345,7 +6045,7 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (59,'Tas Penyimpan Dokumen Penting','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (59,'Tas Penyimpan Dokumen Penting','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -6360,7 +6060,7 @@
       </c>
       <c r="D63" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (60,'Pembalut Charm','SANDANG','Pack','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (60,'Pembalut Charm','SANDANG','Pack','YYYYMMDD');</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -6375,7 +6075,7 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (61,'Pembalut Laurier','SANDANG','Pack','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (61,'Pembalut Laurier','SANDANG','Pack','YYYYMMDD');</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -6390,7 +6090,7 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (62,'Pembalut','SANDANG','Pack','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (62,'Pembalut','SANDANG','Pack','YYYYMMDD');</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -6405,7 +6105,7 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (63,'Pempers','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (63,'Pempers','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -6420,7 +6120,7 @@
       </c>
       <c r="D67" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (64,'Pampers M','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (64,'Pampers M','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -6435,7 +6135,7 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (65,'Pempers L','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (65,'Pempers L','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -6450,7 +6150,7 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (66,'Pampers S','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (66,'Pampers S','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -6465,7 +6165,7 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (67,'Pampers','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (67,'Pampers','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -6480,7 +6180,7 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (68,'Linggis','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (68,'Linggis','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -6495,7 +6195,7 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (69,'Cangkul','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (69,'Cangkul','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -6510,7 +6210,7 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (70,'Skop','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (70,'Skop','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -6525,7 +6225,7 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (71,'Garpu','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (71,'Garpu','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -6540,7 +6240,7 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (72,'Parang','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (72,'Parang','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -6555,7 +6255,7 @@
       </c>
       <c r="D76" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (73,'Helmet Font Brim Ventedorange','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (73,'Helmet Font Brim Ventedorange','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -6570,7 +6270,7 @@
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (74,'Helmet Front Brim Orange','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (74,'Helmet Front Brim Orange','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -6585,7 +6285,7 @@
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (75,'Sarung Tangan Latex Yellow','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (75,'Sarung Tangan Latex Yellow','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -6600,7 +6300,7 @@
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (76,'Sarung Tangan Glove Blue Leather','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (76,'Sarung Tangan Glove Blue Leather','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -6615,7 +6315,7 @@
       </c>
       <c r="D80" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (77,'Sarung Tangan Kain','SANDANG','dos','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (77,'Sarung Tangan Kain','SANDANG','dos','YYYYMMDD');</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -6630,7 +6330,7 @@
       </c>
       <c r="D81" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (78,'Masker','SANDANG','dos','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (78,'Masker','SANDANG','dos','YYYYMMDD');</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -6645,7 +6345,7 @@
       </c>
       <c r="D82" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (79,'Troly','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (79,'Troly','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -6660,7 +6360,7 @@
       </c>
       <c r="D83" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (80,'Hygiene Kit','SANDANG','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (80,'Hygiene Kit','SANDANG','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -6675,7 +6375,7 @@
       </c>
       <c r="D84" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (81,'Sarung ','SANDANG','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (81,'Sarung ','SANDANG','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -6689,8 +6389,8 @@
         <v>328</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" ref="D85:D88" si="2">"INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A85&amp;",'"&amp;B85&amp;"','SANDANG','"&amp;C85&amp;"','[value-5]')"</f>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (82,'Tikar','SANDANG','Pcs','[value-5]')</v>
+        <f t="shared" ref="D85" si="2">"INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A85&amp;",'"&amp;B85&amp;"','SANDANG','"&amp;C85&amp;"','YYYYMMDD');"</f>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (82,'Tikar','SANDANG','Pcs','YYYYMMDD');</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -6709,8 +6409,8 @@
         <v>332</v>
       </c>
       <c r="D88" t="str">
-        <f>"INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A88&amp;",'"&amp;B88&amp;"','MAKANAN DAN MINUMAN','"&amp;C88&amp;"','[value-5]')"</f>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (83,'Air Mineral','MAKANAN DAN MINUMAN','Dus','[value-5]')</v>
+        <f>"INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A88&amp;",'"&amp;B88&amp;"','MAKANAN DAN MINUMAN','"&amp;C88&amp;"','YYYYMMDD');"</f>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (83,'Air Mineral','MAKANAN DAN MINUMAN','Dus','YYYYMMDD');</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -6724,8 +6424,8 @@
         <v>332</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" ref="D89:D111" si="3">"INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A89&amp;",'"&amp;B89&amp;"','MAKANAN DAN MINUMAN','"&amp;C89&amp;"','[value-5]')"</f>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (84,'Air Mineral Botol','MAKANAN DAN MINUMAN','Dus','[value-5]')</v>
+        <f t="shared" ref="D89:D111" si="3">"INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES ("&amp;A89&amp;",'"&amp;B89&amp;"','MAKANAN DAN MINUMAN','"&amp;C89&amp;"','YYYYMMDD');"</f>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (84,'Air Mineral Botol','MAKANAN DAN MINUMAN','Dus','YYYYMMDD');</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -6740,7 +6440,7 @@
       </c>
       <c r="D90" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (85,'Air Mineral Gelas','MAKANAN DAN MINUMAN','Dus','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (85,'Air Mineral Gelas','MAKANAN DAN MINUMAN','Dus','YYYYMMDD');</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -6755,7 +6455,7 @@
       </c>
       <c r="D91" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (86,'Beras','MAKANAN DAN MINUMAN','Kg','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (86,'Beras','MAKANAN DAN MINUMAN','Kg','YYYYMMDD');</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -6770,7 +6470,7 @@
       </c>
       <c r="D92" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (87,'Gula Pasir','MAKANAN DAN MINUMAN','Kg','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (87,'Gula Pasir','MAKANAN DAN MINUMAN','Kg','YYYYMMDD');</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -6785,7 +6485,7 @@
       </c>
       <c r="D93" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (88,'Lauk Pauk','MAKANAN DAN MINUMAN','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (88,'Lauk Pauk','MAKANAN DAN MINUMAN','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -6800,7 +6500,7 @@
       </c>
       <c r="D94" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (89,'Minyak Goreng','MAKANAN DAN MINUMAN','Liter','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (89,'Minyak Goreng','MAKANAN DAN MINUMAN','Liter','YYYYMMDD');</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -6815,7 +6515,7 @@
       </c>
       <c r="D95" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (90,'Mie Instan','MAKANAN DAN MINUMAN','Dus','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (90,'Mie Instan','MAKANAN DAN MINUMAN','Dus','YYYYMMDD');</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -6830,7 +6530,7 @@
       </c>
       <c r="D96" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (91,'Bubur Sun @24','MAKANAN DAN MINUMAN','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (91,'Bubur Sun @24','MAKANAN DAN MINUMAN','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -6845,7 +6545,7 @@
       </c>
       <c r="D97" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (92,'Bubur Sun @24 (Makanan Balita)','MAKANAN DAN MINUMAN','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (92,'Bubur Sun @24 (Makanan Balita)','MAKANAN DAN MINUMAN','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -6860,7 +6560,7 @@
       </c>
       <c r="D98" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (93,'Makanan Balita','MAKANAN DAN MINUMAN','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (93,'Makanan Balita','MAKANAN DAN MINUMAN','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -6875,7 +6575,7 @@
       </c>
       <c r="D99" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (94,'Susu Anak/Balita','MAKANAN DAN MINUMAN','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (94,'Susu Anak/Balita','MAKANAN DAN MINUMAN','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -6890,7 +6590,7 @@
       </c>
       <c r="D100" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (95,'Susu Kaleng','MAKANAN DAN MINUMAN','Kaleng','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (95,'Susu Kaleng','MAKANAN DAN MINUMAN','Kaleng','YYYYMMDD');</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -6905,7 +6605,7 @@
       </c>
       <c r="D101" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (96,'Kecap','MAKANAN DAN MINUMAN','Botol','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (96,'Kecap','MAKANAN DAN MINUMAN','Botol','YYYYMMDD');</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -6920,7 +6620,7 @@
       </c>
       <c r="D102" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (97,'Tambahan Gizi','MAKANAN DAN MINUMAN','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (97,'Tambahan Gizi','MAKANAN DAN MINUMAN','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -6935,7 +6635,7 @@
       </c>
       <c r="D103" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (98,'Saos','MAKANAN DAN MINUMAN','Botol','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (98,'Saos','MAKANAN DAN MINUMAN','Botol','YYYYMMDD');</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -6950,7 +6650,7 @@
       </c>
       <c r="D104" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (99,'Teh Serbuk','MAKANAN DAN MINUMAN','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (99,'Teh Serbuk','MAKANAN DAN MINUMAN','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -6965,7 +6665,7 @@
       </c>
       <c r="D105" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (100,'Teh Celup','MAKANAN DAN MINUMAN','Dus','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (100,'Teh Celup','MAKANAN DAN MINUMAN','Dus','YYYYMMDD');</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -6980,7 +6680,7 @@
       </c>
       <c r="D106" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (101,'Kopi Susu','MAKANAN DAN MINUMAN','Sachet','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (101,'Kopi Susu','MAKANAN DAN MINUMAN','Sachet','YYYYMMDD');</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -6995,7 +6695,7 @@
       </c>
       <c r="D107" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (102,'Kopi Instan','MAKANAN DAN MINUMAN','Sachet','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (102,'Kopi Instan','MAKANAN DAN MINUMAN','Sachet','YYYYMMDD');</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -7010,7 +6710,7 @@
       </c>
       <c r="D108" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (103,'Sarden','MAKANAN DAN MINUMAN','Kaleng','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (103,'Sarden','MAKANAN DAN MINUMAN','Kaleng','YYYYMMDD');</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -7025,7 +6725,7 @@
       </c>
       <c r="D109" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (104,'Siap Saji','MAKANAN DAN MINUMAN','Paket','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (104,'Siap Saji','MAKANAN DAN MINUMAN','Paket','YYYYMMDD');</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -7040,7 +6740,7 @@
       </c>
       <c r="D110" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (105,'Yogurt','MAKANAN DAN MINUMAN','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (105,'Yogurt','MAKANAN DAN MINUMAN','Buah','YYYYMMDD');</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -7055,30 +6755,30 @@
       </c>
       <c r="D111" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO `bantuan`(`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (106,'Daging Kaleng','MAKANAN DAN MINUMAN','Buah','[value-5]')</v>
+        <v>INSERT INTO `bantuan` (`id_bantuan`, `nama_bantuan`, `kategori`, `satuan`, `batch`) VALUES (106,'Daging Kaleng','MAKANAN DAN MINUMAN','Buah','YYYYMMDD');</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="42" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="41" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="38" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B17">
-    <cfRule type="duplicateValues" dxfId="37" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B83">
-    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="35" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84:B85">
-    <cfRule type="duplicateValues" dxfId="34" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87:B111">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7088,7 +6788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -7400,34 +7100,44 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D8:E80"/>
+  <dimension ref="B2:E80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="4:5">
+    <row r="2" spans="2:5">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="8" spans="2:5">
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="4:5">
+    <row r="9" spans="2:5">
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="4:5">
+    <row r="10" spans="2:5">
       <c r="D10" s="14"/>
       <c r="E10" s="10"/>
     </row>
     <row r="80" ht="14.25" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="A26">
-    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7438,7 +7148,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C25"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7447,13 +7157,12 @@
     <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
-  <autoFilter ref="A1:C1"/>
   <conditionalFormatting sqref="C40:C49">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C49">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2023 02 08 16:01
</commit_message>
<xml_diff>
--- a/pengaduan-bpbd.xlsx
+++ b/pengaduan-bpbd.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,15 @@
     <sheet name="BANTUAN" sheetId="3" r:id="rId5"/>
     <sheet name="PELAPORAN" sheetId="6" r:id="rId6"/>
     <sheet name="STOK BANTUAN" sheetId="7" r:id="rId7"/>
-    <sheet name="DAT" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
+    <sheet name="DAT" sheetId="8" r:id="rId9"/>
+    <sheet name="USER_BU" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">BANTUAN!$B$87:$B$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">BANTUAN!$B$87:$B$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">BANTUAN!$B$1:$B$17</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateCount="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="392">
   <si>
     <t>user</t>
   </si>
@@ -1188,12 +1190,30 @@
   </si>
   <si>
     <t>stok_tersedia</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>kepala</t>
+  </si>
+  <si>
+    <t>kudus</t>
+  </si>
+  <si>
+    <t>logistik</t>
+  </si>
+  <si>
+    <t>kajian</t>
+  </si>
+  <si>
+    <t>dyah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1947,6 +1967,168 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="2">
+        <v>893456745</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D2" s="2">
+        <v>893456745</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3" s="2">
+        <v>8934566547</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30">
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4" s="2">
+        <v>893456734</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8934567534</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6" s="2">
+        <v>89778908000</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="F6" s="2">
+        <v>12345</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
@@ -6799,7 +6981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E107"/>
     </sheetView>
   </sheetViews>
@@ -9068,6 +9250,18 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A11"/>
   <sheetViews>

</xml_diff>

<commit_message>
2023 02 22 6:10
</commit_message>
<xml_diff>
--- a/pengaduan-bpbd.xlsx
+++ b/pengaduan-bpbd.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,13 @@
     <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
     <sheet name="DAT" sheetId="8" r:id="rId9"/>
     <sheet name="USER_BU" sheetId="10" r:id="rId10"/>
+    <sheet name="WA" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">BANTUAN!$B$87:$B$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">BANTUAN!$B$1:$B$17</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="447">
   <si>
     <t>user</t>
   </si>
@@ -1208,16 +1209,181 @@
   </si>
   <si>
     <t>dyah</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>review_pelaporan</t>
+  </si>
+  <si>
+    <t>gambar_pelapor</t>
+  </si>
+  <si>
+    <t>gambar_lokasi_bencana</t>
+  </si>
+  <si>
+    <t>gambar_bencana</t>
+  </si>
+  <si>
+    <t>id_petugas_bpbd</t>
+  </si>
+  <si>
+    <t>id_pelapor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPBD KABUPATEN KUDUS </t>
+  </si>
+  <si>
+    <t>Menginformasikan adanya pelaporan dari masyarakat :</t>
+  </si>
+  <si>
+    <t>Untuk pihak yang berkaitan dengan penanganan bencan untuk dapat menjalankan kewajibannya sesuai dengan aturan yang berlaku</t>
+  </si>
+  <si>
+    <t>Terima kasih</t>
+  </si>
+  <si>
+    <t>id_petugas_kajian</t>
+  </si>
+  <si>
+    <t>jumlah_korban</t>
+  </si>
+  <si>
+    <t>keterangan_peninjauan</t>
+  </si>
+  <si>
+    <t>status_peninjauan</t>
+  </si>
+  <si>
+    <t>dusun</t>
+  </si>
+  <si>
+    <t>rt</t>
+  </si>
+  <si>
+    <t>rw</t>
+  </si>
+  <si>
+    <t>jumlah_kk</t>
+  </si>
+  <si>
+    <t>jumlah_rumah</t>
+  </si>
+  <si>
+    <t>sebab</t>
+  </si>
+  <si>
+    <t>akibat</t>
+  </si>
+  <si>
+    <t>upaya_penanganan</t>
+  </si>
+  <si>
+    <t>lain_lain</t>
+  </si>
+  <si>
+    <t>Peninjauan</t>
+  </si>
+  <si>
+    <t>Menginformasikan adanya peninjauan dari petugas kajian bencana sebagai berikut:</t>
+  </si>
+  <si>
+    <t>POSKO</t>
+  </si>
+  <si>
+    <t>id_posko</t>
+  </si>
+  <si>
+    <t>nama_posko</t>
+  </si>
+  <si>
+    <t>jumlah_jiwa</t>
+  </si>
+  <si>
+    <t>balita</t>
+  </si>
+  <si>
+    <t>remaja</t>
+  </si>
+  <si>
+    <t>dewasa</t>
+  </si>
+  <si>
+    <t>lanjut_usia</t>
+  </si>
+  <si>
+    <t>status_posko</t>
+  </si>
+  <si>
+    <t>tanggal_posko</t>
+  </si>
+  <si>
+    <t>tanggal_selesai</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>gambar_posko</t>
+  </si>
+  <si>
+    <t>Menginformasikan adanya posko dari petugas kajian bencana sebagai berikut:</t>
+  </si>
+  <si>
+    <t>id_distribusi</t>
+  </si>
+  <si>
+    <t>tanggal_distribusi</t>
+  </si>
+  <si>
+    <t>keterangan_distribusi</t>
+  </si>
+  <si>
+    <t>status_distribusi</t>
+  </si>
+  <si>
+    <t>bukti_distribusi</t>
+  </si>
+  <si>
+    <t>id_petugas_logistik</t>
+  </si>
+  <si>
+    <t>DISTRIBUSI</t>
+  </si>
+  <si>
+    <t>id_bantuan_distribusi</t>
+  </si>
+  <si>
+    <t>jumlah</t>
+  </si>
+  <si>
+    <t>BANTUAN distribusi</t>
+  </si>
+  <si>
+    <t>Menginformasikan adanya distribusi bantuan dari petugas logistik bencana sebagai berikut:</t>
+  </si>
+  <si>
+    <t>STOK BANTUAN</t>
+  </si>
+  <si>
+    <t>BANTUAN</t>
+  </si>
+  <si>
+    <t>stok</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1270,6 +1436,38 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1312,7 +1510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1342,6 +1540,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1971,8 +2184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2123,6 +2336,1139 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="D1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
+      <c r="D2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="str">
+        <f>CONCATENATE(""". $request['",B5,"'] . ","""")</f>
+        <v>". $request['id_pelaporan'] . "</v>
+      </c>
+      <c r="D5" t="str">
+        <f>CONCATENATE(B5, ":", C5)</f>
+        <v>id_pelaporan:". $request['id_pelaporan'] . "</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C69" si="0">CONCATENATE(""". $request['",B6,"'] . ","""")</f>
+        <v>". $request['id_pelapor'] . "</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" ref="D6:D19" si="1">CONCATENATE(B6, ":", C6)</f>
+        <v>id_pelapor:". $request['id_pelapor'] . "</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_petugas_bpbd'] . "</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>id_petugas_bpbd:". $request['id_petugas_bpbd'] . "</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_bencana'] . "</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>id_bencana:". $request['id_bencana'] . "</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_wilayah'] . "</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>id_wilayah:". $request['id_wilayah'] . "</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['tanggal_pelaporan'] . "</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>tanggal_pelaporan:". $request['tanggal_pelaporan'] . "</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['pelaporan'] . "</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>pelaporan:". $request['pelaporan'] . "</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['link_maps'] . "</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>link_maps:". $request['link_maps'] . "</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['gambar_bencana'] . "</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>gambar_bencana:". $request['gambar_bencana'] . "</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['gambar_lokasi_bencana'] . "</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>gambar_lokasi_bencana:". $request['gambar_lokasi_bencana'] . "</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['gambar_pelapor'] . "</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>gambar_pelapor:". $request['gambar_pelapor'] . "</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['status_pelaporan'] . "</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>status_pelaporan:". $request['status_pelaporan'] . "</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['review_pelaporan'] . "</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>review_pelaporan:". $request['review_pelaporan'] . "</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['created_at'] . "</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>created_at:". $request['created_at'] . "</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['updated_at'] . "</v>
+      </c>
+      <c r="D19" t="str">
+        <f>CONCATENATE(B19, ":", C19)</f>
+        <v>updated_at:". $request['updated_at'] . "</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="D21" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="D22" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="D25" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" t="s">
+        <v>417</v>
+      </c>
+      <c r="D26" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_peninjauan'] . "</v>
+      </c>
+      <c r="D27" t="str">
+        <f>CONCATENATE(B27, ":", C27)</f>
+        <v>id_peninjauan:". $request['id_peninjauan'] . "</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_pelaporan'] . "</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" ref="D28:D47" si="2">CONCATENATE(B28, ":", C28)</f>
+        <v>id_pelaporan:". $request['id_pelaporan'] . "</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_wilayah'] . "</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>id_wilayah:". $request['id_wilayah'] . "</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_bencana'] . "</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>id_bencana:". $request['id_bencana'] . "</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_petugas_kajian'] . "</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>id_petugas_kajian:". $request['id_petugas_kajian'] . "</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['kategori_bencana'] . "</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>kategori_bencana:". $request['kategori_bencana'] . "</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['level_bencana'] . "</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="2"/>
+        <v>level_bencana:". $request['level_bencana'] . "</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['tanggal_peninjauan'] . "</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="2"/>
+        <v>tanggal_peninjauan:". $request['tanggal_peninjauan'] . "</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['jumlah_korban'] . "</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="2"/>
+        <v>jumlah_korban:". $request['jumlah_korban'] . "</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['keterangan_peninjauan'] . "</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="2"/>
+        <v>keterangan_peninjauan:". $request['keterangan_peninjauan'] . "</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['status_peninjauan'] . "</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="2"/>
+        <v>status_peninjauan:". $request['status_peninjauan'] . "</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['bukti_peninjauan'] . "</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="2"/>
+        <v>bukti_peninjauan:". $request['bukti_peninjauan'] . "</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['dusun'] . "</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="2"/>
+        <v>dusun:". $request['dusun'] . "</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['rt'] . "</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="2"/>
+        <v>rt:". $request['rt'] . "</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['rw'] . "</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="2"/>
+        <v>rw:". $request['rw'] . "</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['jumlah_kk'] . "</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="2"/>
+        <v>jumlah_kk:". $request['jumlah_kk'] . "</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['jumlah_rumah'] . "</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="2"/>
+        <v>jumlah_rumah:". $request['jumlah_rumah'] . "</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['sebab'] . "</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="2"/>
+        <v>sebab:". $request['sebab'] . "</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['akibat'] . "</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="2"/>
+        <v>akibat:". $request['akibat'] . "</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['upaya_penanganan'] . "</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="2"/>
+        <v>upaya_penanganan:". $request['upaya_penanganan'] . "</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['lain_lain'] . "</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="2"/>
+        <v>lain_lain:". $request['lain_lain'] . "</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="D49" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="D50" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" t="s">
+        <v>419</v>
+      </c>
+      <c r="D54" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="D55" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_posko'] . "</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" ref="D56:D70" si="3">CONCATENATE(B56, ":", C56)</f>
+        <v>id_posko:". $request['id_posko'] . "</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['id_peninjauan'] . "</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="3"/>
+        <v>id_peninjauan:". $request['id_peninjauan'] . "</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="B58" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['nama_posko'] . "</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="3"/>
+        <v>nama_posko:". $request['nama_posko'] . "</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['jumlah_jiwa'] . "</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="3"/>
+        <v>jumlah_jiwa:". $request['jumlah_jiwa'] . "</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="B60" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['balita'] . "</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="3"/>
+        <v>balita:". $request['balita'] . "</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="B61" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['remaja'] . "</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="3"/>
+        <v>remaja:". $request['remaja'] . "</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['dewasa'] . "</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="3"/>
+        <v>dewasa:". $request['dewasa'] . "</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['lanjut_usia'] . "</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="3"/>
+        <v>lanjut_usia:". $request['lanjut_usia'] . "</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" s="18" t="s">
+        <v>427</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['status_posko'] . "</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="3"/>
+        <v>status_posko:". $request['status_posko'] . "</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="18" t="s">
+        <v>428</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['tanggal_posko'] . "</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="3"/>
+        <v>tanggal_posko:". $request['tanggal_posko'] . "</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="B66" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['tanggal_selesai'] . "</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="3"/>
+        <v>tanggal_selesai:". $request['tanggal_selesai'] . "</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['keterangan'] . "</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="3"/>
+        <v>keterangan:". $request['keterangan'] . "</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['gambar_posko'] . "</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="3"/>
+        <v>gambar_posko:". $request['gambar_posko'] . "</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="0"/>
+        <v>". $request['created_at'] . "</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="3"/>
+        <v>created_at:". $request['created_at'] . "</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" ref="C70" si="4">CONCATENATE(""". $request['",B70,"'] . ","""")</f>
+        <v>". $request['updated_at'] . "</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="3"/>
+        <v>updated_at:". $request['updated_at'] . "</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="D72" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="D73" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="D75" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76" t="s">
+        <v>439</v>
+      </c>
+      <c r="D76" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" ref="C77:C83" si="5">CONCATENATE(""". $request['",B77,"'] . ","""")</f>
+        <v>". $request['id_distribusi'] . "</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" ref="D77:D83" si="6">CONCATENATE(B77, ":", C77)</f>
+        <v>id_distribusi:". $request['id_distribusi'] . "</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="5"/>
+        <v>". $request['id_peninjauan'] . "</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="6"/>
+        <v>id_peninjauan:". $request['id_peninjauan'] . "</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="B79" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="5"/>
+        <v>". $request['tanggal_distribusi'] . "</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="6"/>
+        <v>tanggal_distribusi:". $request['tanggal_distribusi'] . "</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4">
+      <c r="B80" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="5"/>
+        <v>". $request['keterangan_distribusi'] . "</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="6"/>
+        <v>keterangan_distribusi:". $request['keterangan_distribusi'] . "</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="B81" s="18" t="s">
+        <v>436</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="5"/>
+        <v>". $request['status_distribusi'] . "</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="6"/>
+        <v>status_distribusi:". $request['status_distribusi'] . "</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="B82" s="18" t="s">
+        <v>437</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="5"/>
+        <v>". $request['bukti_distribusi'] . "</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="6"/>
+        <v>bukti_distribusi:". $request['bukti_distribusi'] . "</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="B83" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="5"/>
+        <v>". $request['id_petugas_logistik'] . "</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="6"/>
+        <v>id_petugas_logistik:". $request['id_petugas_logistik'] . "</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="D85" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="D86" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" ref="C90:C95" si="7">CONCATENATE(""". $request['",B90,"'] . ","""")</f>
+        <v>". $request['id_bantuan_distribusi'] . "</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" ref="D90:D95" si="8">CONCATENATE(B90, ":", C90)</f>
+        <v>id_bantuan_distribusi:". $request['id_bantuan_distribusi'] . "</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4">
+      <c r="B91" s="17" t="s">
+        <v>433</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="7"/>
+        <v>". $request['id_distribusi'] . "</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="8"/>
+        <v>id_distribusi:". $request['id_distribusi'] . "</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="7"/>
+        <v>". $request['id_stok_bantuan'] . "</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="8"/>
+        <v>id_stok_bantuan:". $request['id_stok_bantuan'] . "</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="7"/>
+        <v>". $request['jumlah'] . "</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="8"/>
+        <v>jumlah:". $request['jumlah'] . "</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="7"/>
+        <v>". $request['satuan'] . "</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="8"/>
+        <v>satuan:". $request['satuan'] . "</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="B95" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="7"/>
+        <v>". $request['batch'] . "</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="8"/>
+        <v>batch:". $request['batch'] . "</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="B99" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4">
+      <c r="B100" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" ref="C100:C107" si="9">CONCATENATE(""". $request['",B100,"'] . ","""")</f>
+        <v>". $request['id_stok_bantuan'] . "</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" ref="D100:D107" si="10">CONCATENATE(B100, ":", C100)</f>
+        <v>id_stok_bantuan:". $request['id_stok_bantuan'] . "</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4">
+      <c r="B101" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="9"/>
+        <v>". $request['id_bantuan'] . "</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="10"/>
+        <v>id_bantuan:". $request['id_bantuan'] . "</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4">
+      <c r="B102" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="9"/>
+        <v>". $request['tanggal_masuk'] . "</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="10"/>
+        <v>tanggal_masuk:". $request['tanggal_masuk'] . "</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4">
+      <c r="B103" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="9"/>
+        <v>". $request['tanggal_kadaluarsa'] . "</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="10"/>
+        <v>tanggal_kadaluarsa:". $request['tanggal_kadaluarsa'] . "</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4">
+      <c r="B104" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="9"/>
+        <v>". $request['stok_masuk'] . "</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="10"/>
+        <v>stok_masuk:". $request['stok_masuk'] . "</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4">
+      <c r="B105" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="9"/>
+        <v>". $request['stok_tersedia'] . "</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="10"/>
+        <v>stok_tersedia:". $request['stok_tersedia'] . "</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4">
+      <c r="B106" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="9"/>
+        <v>". $request['batch'] . "</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="10"/>
+        <v>batch:". $request['batch'] . "</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4">
+      <c r="B107" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="9"/>
+        <v>". $request['satuan'] . "</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="10"/>
+        <v>satuan:". $request['satuan'] . "</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4">
+      <c r="B110" s="18" t="s">
+        <v>445</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" ref="C108:C115" si="11">CONCATENATE(""". $request['",B110,"'] . ","""")</f>
+        <v>". $request['BANTUAN'] . "</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" ref="D108:D115" si="12">CONCATENATE(B110, ":", C110)</f>
+        <v>BANTUAN:". $request['BANTUAN'] . "</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="B111" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="11"/>
+        <v>". $request['id_bantuan'] . "</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="12"/>
+        <v>id_bantuan:". $request['id_bantuan'] . "</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4">
+      <c r="B112" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C112" t="str">
+        <f t="shared" si="11"/>
+        <v>". $request['nama_bantuan'] . "</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="12"/>
+        <v>nama_bantuan:". $request['nama_bantuan'] . "</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4">
+      <c r="B113" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C113" t="str">
+        <f t="shared" si="11"/>
+        <v>". $request['kategori'] . "</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="12"/>
+        <v>kategori:". $request['kategori'] . "</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4">
+      <c r="B114" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C114" t="str">
+        <f t="shared" si="11"/>
+        <v>". $request['satuan'] . "</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="12"/>
+        <v>satuan:". $request['satuan'] . "</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4">
+      <c r="B115" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="C115" t="str">
+        <f t="shared" si="11"/>
+        <v>". $request['stok'] . "</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="12"/>
+        <v>stok:". $request['stok'] . "</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2023 02 22 11:32
</commit_message>
<xml_diff>
--- a/pengaduan-bpbd.xlsx
+++ b/pengaduan-bpbd.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="10"/>
   </bookViews>
@@ -1379,7 +1379,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -2346,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2389,7 +2389,7 @@
         <v>". $request['id_pelapor'] . "</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" ref="D6:D19" si="1">CONCATENATE(B6, ":", C6)</f>
+        <f t="shared" ref="D6:D18" si="1">CONCATENATE(B6, ":", C6)</f>
         <v>id_pelapor:". $request['id_pelapor'] . "</v>
       </c>
     </row>
@@ -3397,11 +3397,11 @@
         <v>445</v>
       </c>
       <c r="C110" t="str">
-        <f t="shared" ref="C108:C115" si="11">CONCATENATE(""". $request['",B110,"'] . ","""")</f>
+        <f t="shared" ref="C110:C115" si="11">CONCATENATE(""". $request['",B110,"'] . ","""")</f>
         <v>". $request['BANTUAN'] . "</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" ref="D108:D115" si="12">CONCATENATE(B110, ":", C110)</f>
+        <f t="shared" ref="D110:D115" si="12">CONCATENATE(B110, ":", C110)</f>
         <v>BANTUAN:". $request['BANTUAN'] . "</v>
       </c>
     </row>

</xml_diff>